<commit_message>
Update demo region databooks
Demo region 1 now has double the stunting prevalence of region 2; demo region 3 has half the stunting prevalence of region 2
</commit_message>
<xml_diff>
--- a/inputs/demo_region1_input.xlsx
+++ b/inputs/demo_region1_input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961"/>
+    <workbookView xWindow="-38400" yWindow="-21144" windowWidth="38400" windowHeight="21144" tabRatio="961" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4790,18 +4790,18 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="14.453125" style="12"/>
+    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="14.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4812,14 +4812,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>193</v>
@@ -4828,7 +4828,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>192</v>
@@ -4837,7 +4837,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -4906,7 +4906,7 @@
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
         <v>129</v>
       </c>
@@ -5047,7 +5047,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -5251,15 +5251,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.81640625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.453125" style="35"/>
+    <col min="2" max="2" width="47.77734375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -5400,13 +5400,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="11.453125" style="35"/>
+    <col min="1" max="1" width="30.109375" style="35" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -5498,7 +5498,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -5612,19 +5612,19 @@
       <selection activeCell="C29" activeCellId="3" sqref="C2:O12 C14:O21 C23:O27 C29:O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -6186,7 +6186,7 @@
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>86</v>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>187</v>
@@ -6331,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>208</v>
@@ -6567,7 +6567,7 @@
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
         <v>37</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -7326,7 +7326,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
@@ -7364,16 +7364,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="35" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" style="35"/>
-    <col min="5" max="5" width="17.453125" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="35"/>
+    <col min="1" max="1" width="33.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="35"/>
+    <col min="5" max="5" width="17.44140625" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>163</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>157</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>156</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>155</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>153</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>152</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>151</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>150</v>
       </c>
@@ -7573,20 +7573,20 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" style="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" style="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.08984375" style="55" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.36328125" style="55" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.90625" style="55" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="16.08984375" style="55"/>
+    <col min="6" max="7" width="13.109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.33203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.88671875" style="55" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.109375" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>33</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>31</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="52" t="s">
         <v>149</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="52" t="s">
         <v>173</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="52" t="s">
         <v>198</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="52" t="s">
         <v>199</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="s">
         <v>195</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>136</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="52" t="s">
         <v>137</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="52" t="s">
         <v>84</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52" t="s">
         <v>58</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="52" t="s">
         <v>67</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52" t="s">
         <v>28</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="52" t="s">
         <v>85</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="52" t="s">
         <v>60</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="52"/>
       <c r="C16" s="91"/>
       <c r="D16" s="91"/>
@@ -8268,7 +8268,7 @@
       <c r="N16" s="91"/>
       <c r="O16" s="91"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56" t="s">
         <v>32</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="56"/>
       <c r="B18" s="52" t="s">
         <v>86</v>
@@ -8360,7 +8360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="92" t="s">
         <v>187</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="92" t="s">
         <v>208</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="93" t="s">
         <v>57</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="52" t="s">
         <v>88</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="52" t="s">
         <v>87</v>
       </c>
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="52" t="s">
         <v>59</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="52"/>
       <c r="C25" s="91"/>
       <c r="D25" s="91"/>
@@ -8640,7 +8640,7 @@
       <c r="N25" s="91"/>
       <c r="O25" s="91"/>
     </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56" t="s">
         <v>37</v>
       </c>
@@ -8688,7 +8688,7 @@
       </c>
       <c r="P26" s="94"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="59" t="s">
         <v>188</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="56"/>
       <c r="B28" s="59" t="s">
         <v>207</v>
@@ -8777,7 +8777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="59" t="s">
         <v>189</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="59" t="s">
         <v>190</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="52"/>
       <c r="C31" s="95"/>
       <c r="D31" s="95"/>
@@ -8881,7 +8881,7 @@
       <c r="N31" s="91"/>
       <c r="O31" s="91"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
         <v>35</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="52" t="s">
         <v>64</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="52" t="s">
         <v>62</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="52" t="s">
         <v>47</v>
       </c>
@@ -9060,7 +9060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="52" t="s">
         <v>34</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="97"/>
       <c r="B37" s="52" t="s">
         <v>83</v>
@@ -9149,7 +9149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="52" t="s">
         <v>82</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="52" t="s">
         <v>81</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="52" t="s">
         <v>79</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="52" t="s">
         <v>80</v>
       </c>
@@ -9342,22 +9342,22 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -10088,22 +10088,22 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>217</v>
       </c>
@@ -10462,15 +10462,15 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.08984375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="35" customWidth="1"/>
     <col min="2" max="2" width="15" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="12.81640625" style="35"/>
+    <col min="3" max="3" width="14.6640625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>218</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>219</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="101" t="s">
         <v>172</v>
       </c>
@@ -10857,7 +10857,7 @@
       <c r="G18" s="102"/>
       <c r="H18" s="102"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>220</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="101" t="s">
         <v>172</v>
       </c>
@@ -11215,7 +11215,7 @@
       <c r="G35" s="102"/>
       <c r="H35" s="102"/>
     </row>
-    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="103" t="s">
         <v>221</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="104" t="s">
         <v>172</v>
       </c>
@@ -11569,6 +11569,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11578,12 +11584,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11601,14 +11601,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="12" customWidth="1"/>
-    <col min="2" max="9" width="16.81640625" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="14.453125" style="12"/>
+    <col min="1" max="1" width="8.44140625" style="12" customWidth="1"/>
+    <col min="2" max="9" width="16.77734375" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="14.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -12697,22 +12697,22 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="35" customWidth="1"/>
     <col min="5" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="16.08984375" style="35"/>
+    <col min="7" max="16384" width="16.109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="106" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="106" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="105" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="107"/>
       <c r="C2" s="108" t="s">
         <v>26</v>
@@ -12727,7 +12727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>223</v>
       </c>
@@ -12811,7 +12811,7 @@
       <c r="E8" s="100"/>
       <c r="F8" s="100"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>224</v>
       </c>
@@ -12836,7 +12836,7 @@
       <c r="F10" s="100"/>
       <c r="G10" s="117"/>
     </row>
-    <row r="11" spans="1:7" s="106" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="106" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="105" t="s">
         <v>225</v>
       </c>
@@ -12846,7 +12846,7 @@
       <c r="F11" s="119"/>
       <c r="G11" s="120"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>226</v>
       </c>
@@ -12910,7 +12910,7 @@
       </c>
       <c r="G15" s="117"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="121"/>
       <c r="C16" s="122"/>
@@ -12919,7 +12919,7 @@
       <c r="F16" s="100"/>
       <c r="G16" s="117"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>230</v>
       </c>
@@ -13073,7 +13073,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="121"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
     </row>
   </sheetData>
@@ -13094,23 +13094,23 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="35" customWidth="1"/>
-    <col min="4" max="8" width="14.81640625" style="35" customWidth="1"/>
-    <col min="9" max="12" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="16.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="27.21875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="35" customWidth="1"/>
+    <col min="4" max="8" width="14.77734375" style="35" customWidth="1"/>
+    <col min="9" max="12" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="106" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="106" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="105" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="126" t="s">
         <v>212</v>
       </c>
@@ -13144,7 +13144,7 @@
       <c r="O2" s="128"/>
       <c r="P2" s="128"/>
     </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="40"/>
       <c r="B3" s="35" t="s">
         <v>71</v>
@@ -13577,7 +13577,7 @@
       <c r="O17" s="126"/>
       <c r="P17" s="126"/>
     </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="43" t="s">
         <v>237</v>
       </c>
@@ -13835,12 +13835,12 @@
       <c r="O26" s="126"/>
       <c r="P26" s="126"/>
     </row>
-    <row r="28" spans="1:16" s="106" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="106" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="105" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="129" t="s">
         <v>239</v>
       </c>
@@ -13874,7 +13874,7 @@
       <c r="O29" s="128"/>
       <c r="P29" s="128"/>
     </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="35" t="s">
         <v>71</v>
@@ -14569,12 +14569,12 @@
       <c r="C54" s="43"/>
       <c r="D54" s="43"/>
     </row>
-    <row r="55" spans="1:16" s="106" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" s="106" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="105" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="129" t="s">
         <v>70</v>
       </c>
@@ -14602,7 +14602,7 @@
       <c r="O56" s="128"/>
       <c r="P56" s="128"/>
     </row>
-    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="35" t="s">
         <v>38</v>
@@ -14748,12 +14748,12 @@
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
     </row>
-    <row r="64" spans="1:16" s="106" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" s="106" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="105" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="129" t="s">
         <v>24</v>
       </c>
@@ -14787,7 +14787,7 @@
       <c r="O65" s="128"/>
       <c r="P65" s="128"/>
     </row>
-    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="133"/>
       <c r="B66" s="35" t="s">
         <v>73</v>
@@ -15823,12 +15823,12 @@
       <c r="O101" s="126"/>
       <c r="P101" s="126"/>
     </row>
-    <row r="103" spans="1:16" s="106" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" s="106" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="105" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A104" s="129" t="s">
         <v>71</v>
       </c>
@@ -15862,7 +15862,7 @@
       <c r="O104" s="128"/>
       <c r="P104" s="128"/>
     </row>
-    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="36"/>
       <c r="C105" s="43" t="s">
@@ -15976,7 +15976,7 @@
       <c r="O108" s="126"/>
       <c r="P108" s="126"/>
     </row>
-    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
     </row>
   </sheetData>
@@ -15997,24 +15997,24 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="44.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="35" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="35" customWidth="1"/>
     <col min="6" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="7" max="7" width="13.6640625" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="105" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="133" t="s">
         <v>25</v>
       </c>
@@ -16055,7 +16055,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="125" t="s">
         <v>251</v>
@@ -16076,7 +16076,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="110" t="s">
         <v>252</v>
       </c>
@@ -16149,12 +16149,12 @@
       <c r="F9" s="125"/>
       <c r="G9" s="125"/>
     </row>
-    <row r="10" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="105" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="110"/>
       <c r="B11" s="121" t="s">
         <v>195</v>
@@ -16175,16 +16175,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
       <c r="B12" s="121"/>
     </row>
-    <row r="13" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="105" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="133" t="s">
         <v>239</v>
       </c>
@@ -16207,7 +16207,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="125" t="s">
         <v>256</v>
@@ -16228,7 +16228,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="133" t="s">
         <v>70</v>
       </c>
@@ -16252,12 +16252,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="106" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="105" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="110" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="110" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="56" t="s">
         <v>49</v>
       </c>
@@ -16307,16 +16307,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" style="35" customWidth="1"/>
-    <col min="2" max="6" width="16.08984375" style="35"/>
-    <col min="7" max="7" width="17.1796875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="16.08984375" style="35"/>
+    <col min="1" max="1" width="52.21875" style="35" customWidth="1"/>
+    <col min="2" max="6" width="16.109375" style="35"/>
+    <col min="7" max="7" width="17.21875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="16.109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="127" t="s">
         <v>69</v>
       </c>
@@ -16586,15 +16586,15 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="15" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="12.81640625" style="35"/>
+    <col min="16" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="109" t="s">
@@ -16637,7 +16637,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>261</v>
       </c>
@@ -17082,7 +17082,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
         <v>137</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>262</v>
       </c>
@@ -17382,15 +17382,15 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" style="35" customWidth="1"/>
-    <col min="3" max="7" width="15.54296875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="21.33203125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" style="35" customWidth="1"/>
+    <col min="3" max="7" width="15.5546875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
       <c r="B1" s="127"/>
       <c r="C1" s="40" t="s">
@@ -17409,7 +17409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>263</v>
       </c>
@@ -17434,7 +17434,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>264</v>
       </c>
@@ -17483,20 +17483,20 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="52" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="52" customWidth="1"/>
     <col min="4" max="4" width="15" style="35" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="35"/>
-    <col min="8" max="8" width="17.54296875" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="12.81640625" style="35"/>
+    <col min="5" max="5" width="13.6640625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="35"/>
+    <col min="8" max="8" width="17.5546875" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -18613,16 +18613,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" style="35" customWidth="1"/>
-    <col min="4" max="7" width="17.1796875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="2" max="2" width="27.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="35" customWidth="1"/>
+    <col min="4" max="7" width="17.21875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="127" t="s">
         <v>69</v>
       </c>
@@ -18789,14 +18789,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -18807,7 +18807,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -18906,7 +18906,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -19112,7 +19112,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -19224,17 +19224,17 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -19267,23 +19267,23 @@
       </c>
       <c r="C2" s="76">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
-        <v>0.54471569980476653</v>
+        <v>0.35381383595273463</v>
       </c>
       <c r="D2" s="76">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE), "")</f>
-        <v>0.54471569980476653</v>
+        <v>0.35381383595273463</v>
       </c>
       <c r="E2" s="76">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE), "")</f>
-        <v>0.44982829694488635</v>
+        <v>0.2418969293934905</v>
       </c>
       <c r="F2" s="76">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE), "")</f>
-        <v>0.24457139941017503</v>
+        <v>4.4626605907023831E-2</v>
       </c>
       <c r="G2" s="76">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE), "")</f>
-        <v>0.23269074767298425</v>
+        <v>3.6196050479196717E-2</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -19293,23 +19293,23 @@
       </c>
       <c r="C3" s="76">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
-        <v>0.32228430019523346</v>
+        <v>0.38018616404726535</v>
       </c>
       <c r="D3" s="76">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
-        <v>0.32228430019523346</v>
+        <v>0.38018616404726535</v>
       </c>
       <c r="E3" s="76">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
-        <v>0.35908666207150708</v>
+        <v>0.37593298863929642</v>
       </c>
       <c r="F3" s="76">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
-        <v>0.37651189492768178</v>
+        <v>0.19753998276868978</v>
       </c>
       <c r="G3" s="76">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
-        <v>0.37372365733745416</v>
+        <v>0.17663275954168012</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -19318,19 +19318,19 @@
         <v>116</v>
       </c>
       <c r="C4" s="77">
-        <v>8.7000000000000008E-2</v>
+        <v>0.17400000000000002</v>
       </c>
       <c r="D4" s="77">
-        <v>8.7000000000000008E-2</v>
+        <v>0.17400000000000002</v>
       </c>
       <c r="E4" s="77">
-        <v>0.13443032786885245</v>
+        <v>0.2688606557377049</v>
       </c>
       <c r="F4" s="77">
-        <v>0.24673186710341602</v>
+        <v>0.49346373420683204</v>
       </c>
       <c r="G4" s="77">
-        <v>0.25929610299234518</v>
+        <v>0.51859220598469036</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -19339,19 +19339,19 @@
         <v>119</v>
       </c>
       <c r="C5" s="77">
-        <v>4.5999999999999999E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="D5" s="77">
-        <v>4.5999999999999999E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E5" s="77">
-        <v>5.6654713114754097E-2</v>
+        <v>0.11330942622950819</v>
       </c>
       <c r="F5" s="77">
-        <v>0.13218483855872717</v>
+        <v>0.26436967711745435</v>
       </c>
       <c r="G5" s="77">
-        <v>0.13428949199721643</v>
+        <v>0.26857898399443286</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -19655,13 +19655,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="7" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -19791,13 +19791,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -19996,15 +19996,15 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="35" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.453125" style="35"/>
+    <col min="2" max="2" width="19.109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>178</v>
       </c>
@@ -20021,7 +20021,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>173</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="80"/>
     </row>
-    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>198</v>
       </c>
@@ -20173,7 +20173,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="80"/>
     </row>
-    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>199</v>
       </c>
@@ -20272,15 +20272,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>164</v>
       </c>
@@ -20294,7 +20294,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>69</v>
       </c>
@@ -20306,7 +20306,7 @@
       </c>
       <c r="D2" s="80"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
         <v>185</v>
       </c>
@@ -20335,17 +20335,17 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="52" customWidth="1"/>
     <col min="2" max="2" width="20" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="32.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.453125" style="35"/>
+    <col min="3" max="3" width="20.44140625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>69</v>
       </c>
@@ -20635,7 +20635,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Works with no differences when running demo region1
</commit_message>
<xml_diff>
--- a/inputs/demo_region1_input.xlsx
+++ b/inputs/demo_region1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB9EC21-1B9E-4F2A-A366-B22DA600CC03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362D4C81-5E3A-4DAA-898D-0080FD5A0AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="2" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="Programs target population" sheetId="21" r:id="rId13"/>
     <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId14"/>
     <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
-    <sheet name="Programs impacted population" sheetId="62" state="hidden" r:id="rId16"/>
+    <sheet name="Programs impacted population" sheetId="62" r:id="rId16"/>
     <sheet name="Program risk areas" sheetId="63" r:id="rId17"/>
     <sheet name="Population risk areas" sheetId="64" state="hidden" r:id="rId18"/>
     <sheet name="IYCF odds ratios" sheetId="65" state="hidden" r:id="rId19"/>
@@ -493,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="270">
   <si>
     <t>year</t>
   </si>
@@ -2648,15 +2648,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyBorder="1"/>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="728">
@@ -5312,7 +5312,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>187</v>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="C2" s="78"/>
     </row>
-    <row r="3" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
         <v>208</v>
       </c>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="C3" s="78"/>
     </row>
-    <row r="4" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="82" t="s">
         <v>58</v>
       </c>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="C4" s="78"/>
     </row>
-    <row r="5" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="82" t="s">
         <v>137</v>
       </c>
@@ -5348,77 +5348,77 @@
       </c>
       <c r="C5" s="78"/>
     </row>
-    <row r="6" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="82"/>
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
     </row>
-    <row r="7" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="82"/>
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
     </row>
-    <row r="8" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="82"/>
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
     </row>
-    <row r="9" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="82"/>
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
     </row>
-    <row r="10" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="82"/>
       <c r="B10" s="83"/>
       <c r="C10" s="83"/>
     </row>
-    <row r="11" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="84"/>
       <c r="B11" s="83"/>
       <c r="C11" s="83"/>
     </row>
-    <row r="12" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="84"/>
       <c r="B12" s="83"/>
       <c r="C12" s="83"/>
     </row>
-    <row r="13" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="84"/>
       <c r="B13" s="83"/>
       <c r="C13" s="83"/>
     </row>
-    <row r="14" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="84"/>
       <c r="B14" s="83"/>
       <c r="C14" s="83"/>
     </row>
-    <row r="15" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
       <c r="B15" s="83"/>
       <c r="C15" s="83"/>
     </row>
-    <row r="16" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
       <c r="B16" s="83"/>
       <c r="C16" s="83"/>
     </row>
-    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="84"/>
       <c r="B17" s="83"/>
       <c r="C17" s="83"/>
     </row>
-    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="84"/>
       <c r="B18" s="83"/>
       <c r="C18" s="83"/>
     </row>
-    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="82"/>
       <c r="B19" s="83"/>
       <c r="C19" s="83"/>
     </row>
-    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="82"/>
       <c r="B20" s="83"/>
       <c r="C20" s="83"/>
@@ -5453,74 +5453,74 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
     </row>
-    <row r="12" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
-    <row r="13" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
     </row>
-    <row r="14" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
     </row>
-    <row r="15" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="48"/>
     </row>
-    <row r="16" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
     </row>
-    <row r="18" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
     </row>
-    <row r="19" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
     </row>
   </sheetData>
@@ -5651,7 +5651,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="C10" s="85">
         <v>0</v>
@@ -7401,7 +7401,7 @@
       <c r="B40" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="w0Bxihd6J/weql6Phqk6S9/qrXvqWZ4a5y3YpmKACf5GM4dfICpmTrs1srgLFetCu5O81h6jYFRILMMk9VH9Ow==" saltValue="z+F0dItCpyRiY0ZZ8MfzzQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uzFiVlZAFzOqZjKQI0Mm+cttFWZQLq/o0gfs9tyiNeLf1Tcvb6JNmIjcDFwiFL9i1taMiJ9jgbSaXLYDkoXwuw==" saltValue="v687blzXd7cIUYGRLRo45w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:O22">
     <sortCondition ref="B15:B22"/>
   </sortState>
@@ -7657,10 +7657,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8212,13 +8212,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="52" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="C13" s="88">
         <v>0</v>
       </c>
       <c r="D13" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="88">
         <v>1</v>
@@ -8256,13 +8256,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="52" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="C14" s="88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="88">
         <v>1</v>
@@ -8300,159 +8300,159 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="88">
+        <v>1</v>
+      </c>
+      <c r="D15" s="88">
+        <v>1</v>
+      </c>
+      <c r="E15" s="88">
+        <v>1</v>
+      </c>
+      <c r="F15" s="88">
+        <v>1</v>
+      </c>
+      <c r="G15" s="88">
+        <v>1</v>
+      </c>
+      <c r="H15" s="88">
+        <v>0</v>
+      </c>
+      <c r="I15" s="88">
+        <v>0</v>
+      </c>
+      <c r="J15" s="88">
+        <v>0</v>
+      </c>
+      <c r="K15" s="88">
+        <v>0</v>
+      </c>
+      <c r="L15" s="88">
+        <v>0</v>
+      </c>
+      <c r="M15" s="88">
+        <v>0</v>
+      </c>
+      <c r="N15" s="88">
+        <v>0</v>
+      </c>
+      <c r="O15" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="88">
-        <v>0</v>
-      </c>
-      <c r="D15" s="88">
-        <v>0</v>
-      </c>
-      <c r="E15" s="88">
-        <v>1</v>
-      </c>
-      <c r="F15" s="88">
-        <v>1</v>
-      </c>
-      <c r="G15" s="88">
-        <v>1</v>
-      </c>
-      <c r="H15" s="88">
-        <v>0</v>
-      </c>
-      <c r="I15" s="88">
-        <v>0</v>
-      </c>
-      <c r="J15" s="88">
-        <v>0</v>
-      </c>
-      <c r="K15" s="88">
-        <v>0</v>
-      </c>
-      <c r="L15" s="88">
-        <v>0</v>
-      </c>
-      <c r="M15" s="88">
-        <v>0</v>
-      </c>
-      <c r="N15" s="88">
-        <v>0</v>
-      </c>
-      <c r="O15" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="52"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
+      <c r="C16" s="88">
+        <v>0</v>
+      </c>
+      <c r="D16" s="88">
+        <v>0</v>
+      </c>
+      <c r="E16" s="88">
+        <v>1</v>
+      </c>
+      <c r="F16" s="88">
+        <v>1</v>
+      </c>
+      <c r="G16" s="88">
+        <v>1</v>
+      </c>
+      <c r="H16" s="88">
+        <v>0</v>
+      </c>
+      <c r="I16" s="88">
+        <v>0</v>
+      </c>
+      <c r="J16" s="88">
+        <v>0</v>
+      </c>
+      <c r="K16" s="88">
+        <v>0</v>
+      </c>
+      <c r="L16" s="88">
+        <v>0</v>
+      </c>
+      <c r="M16" s="88">
+        <v>0</v>
+      </c>
+      <c r="N16" s="88">
+        <v>0</v>
+      </c>
+      <c r="O16" s="88">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B18" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="88">
-        <v>0</v>
-      </c>
-      <c r="D17" s="88">
-        <v>0</v>
-      </c>
-      <c r="E17" s="88">
-        <v>0</v>
-      </c>
-      <c r="F17" s="88">
-        <v>0</v>
-      </c>
-      <c r="G17" s="88">
-        <v>0</v>
-      </c>
-      <c r="H17" s="88">
-        <v>1</v>
-      </c>
-      <c r="I17" s="88">
-        <v>1</v>
-      </c>
-      <c r="J17" s="88">
-        <v>1</v>
-      </c>
-      <c r="K17" s="88">
-        <v>1</v>
-      </c>
-      <c r="L17" s="88">
-        <v>0</v>
-      </c>
-      <c r="M17" s="88">
-        <v>0</v>
-      </c>
-      <c r="N17" s="88">
-        <v>0</v>
-      </c>
-      <c r="O17" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
-      <c r="B18" s="52" t="s">
+      <c r="C18" s="88">
+        <v>0</v>
+      </c>
+      <c r="D18" s="88">
+        <v>0</v>
+      </c>
+      <c r="E18" s="88">
+        <v>0</v>
+      </c>
+      <c r="F18" s="88">
+        <v>0</v>
+      </c>
+      <c r="G18" s="88">
+        <v>0</v>
+      </c>
+      <c r="H18" s="88">
+        <v>1</v>
+      </c>
+      <c r="I18" s="88">
+        <v>1</v>
+      </c>
+      <c r="J18" s="88">
+        <v>1</v>
+      </c>
+      <c r="K18" s="88">
+        <v>1</v>
+      </c>
+      <c r="L18" s="88">
+        <v>0</v>
+      </c>
+      <c r="M18" s="88">
+        <v>0</v>
+      </c>
+      <c r="N18" s="88">
+        <v>0</v>
+      </c>
+      <c r="O18" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="56"/>
+      <c r="B19" s="52" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="88">
-        <v>0</v>
-      </c>
-      <c r="D18" s="88">
-        <v>0</v>
-      </c>
-      <c r="E18" s="88">
-        <v>0</v>
-      </c>
-      <c r="F18" s="88">
-        <v>0</v>
-      </c>
-      <c r="G18" s="88">
-        <v>0</v>
-      </c>
-      <c r="H18" s="88">
-        <v>1</v>
-      </c>
-      <c r="I18" s="88">
-        <v>1</v>
-      </c>
-      <c r="J18" s="88">
-        <v>1</v>
-      </c>
-      <c r="K18" s="88">
-        <v>1</v>
-      </c>
-      <c r="L18" s="88">
-        <v>0</v>
-      </c>
-      <c r="M18" s="88">
-        <v>0</v>
-      </c>
-      <c r="N18" s="88">
-        <v>0</v>
-      </c>
-      <c r="O18" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="90" t="s">
-        <v>187</v>
       </c>
       <c r="C19" s="88">
         <v>0</v>
@@ -8496,95 +8496,95 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="90" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="88">
+        <v>0</v>
+      </c>
+      <c r="D20" s="88">
+        <v>0</v>
+      </c>
+      <c r="E20" s="88">
+        <v>0</v>
+      </c>
+      <c r="F20" s="88">
+        <v>0</v>
+      </c>
+      <c r="G20" s="88">
+        <v>0</v>
+      </c>
+      <c r="H20" s="88">
+        <v>1</v>
+      </c>
+      <c r="I20" s="88">
+        <v>1</v>
+      </c>
+      <c r="J20" s="88">
+        <v>1</v>
+      </c>
+      <c r="K20" s="88">
+        <v>1</v>
+      </c>
+      <c r="L20" s="88">
+        <v>0</v>
+      </c>
+      <c r="M20" s="88">
+        <v>0</v>
+      </c>
+      <c r="N20" s="88">
+        <v>0</v>
+      </c>
+      <c r="O20" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="C20" s="88">
-        <v>0</v>
-      </c>
-      <c r="D20" s="88">
-        <v>0</v>
-      </c>
-      <c r="E20" s="88">
-        <v>0</v>
-      </c>
-      <c r="F20" s="88">
-        <v>0</v>
-      </c>
-      <c r="G20" s="88">
-        <v>0</v>
-      </c>
-      <c r="H20" s="88">
-        <v>1</v>
-      </c>
-      <c r="I20" s="88">
-        <v>1</v>
-      </c>
-      <c r="J20" s="88">
-        <v>1</v>
-      </c>
-      <c r="K20" s="88">
-        <v>1</v>
-      </c>
-      <c r="L20" s="88">
-        <v>0</v>
-      </c>
-      <c r="M20" s="88">
-        <v>0</v>
-      </c>
-      <c r="N20" s="88">
-        <v>0</v>
-      </c>
-      <c r="O20" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="91" t="s">
+      <c r="C21" s="88">
+        <v>0</v>
+      </c>
+      <c r="D21" s="88">
+        <v>0</v>
+      </c>
+      <c r="E21" s="88">
+        <v>0</v>
+      </c>
+      <c r="F21" s="88">
+        <v>0</v>
+      </c>
+      <c r="G21" s="88">
+        <v>0</v>
+      </c>
+      <c r="H21" s="88">
+        <v>1</v>
+      </c>
+      <c r="I21" s="88">
+        <v>1</v>
+      </c>
+      <c r="J21" s="88">
+        <v>1</v>
+      </c>
+      <c r="K21" s="88">
+        <v>1</v>
+      </c>
+      <c r="L21" s="88">
+        <v>0</v>
+      </c>
+      <c r="M21" s="88">
+        <v>0</v>
+      </c>
+      <c r="N21" s="88">
+        <v>0</v>
+      </c>
+      <c r="O21" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="91" t="s">
         <v>57</v>
-      </c>
-      <c r="C21" s="88">
-        <v>0</v>
-      </c>
-      <c r="D21" s="88">
-        <v>0</v>
-      </c>
-      <c r="E21" s="88">
-        <v>0</v>
-      </c>
-      <c r="F21" s="88">
-        <v>0</v>
-      </c>
-      <c r="G21" s="88">
-        <v>0</v>
-      </c>
-      <c r="H21" s="88">
-        <v>1</v>
-      </c>
-      <c r="I21" s="88">
-        <v>1</v>
-      </c>
-      <c r="J21" s="88">
-        <v>1</v>
-      </c>
-      <c r="K21" s="88">
-        <v>1</v>
-      </c>
-      <c r="L21" s="88">
-        <v>0</v>
-      </c>
-      <c r="M21" s="88">
-        <v>0</v>
-      </c>
-      <c r="N21" s="88">
-        <v>0</v>
-      </c>
-      <c r="O21" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="52" t="s">
-        <v>88</v>
       </c>
       <c r="C22" s="88">
         <v>0</v>
@@ -8628,7 +8628,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="52" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="88">
         <v>0</v>
@@ -8672,204 +8672,204 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="88">
+        <v>0</v>
+      </c>
+      <c r="D24" s="88">
+        <v>0</v>
+      </c>
+      <c r="E24" s="88">
+        <v>0</v>
+      </c>
+      <c r="F24" s="88">
+        <v>0</v>
+      </c>
+      <c r="G24" s="88">
+        <v>0</v>
+      </c>
+      <c r="H24" s="88">
+        <v>1</v>
+      </c>
+      <c r="I24" s="88">
+        <v>1</v>
+      </c>
+      <c r="J24" s="88">
+        <v>1</v>
+      </c>
+      <c r="K24" s="88">
+        <v>1</v>
+      </c>
+      <c r="L24" s="88">
+        <v>0</v>
+      </c>
+      <c r="M24" s="88">
+        <v>0</v>
+      </c>
+      <c r="N24" s="88">
+        <v>0</v>
+      </c>
+      <c r="O24" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="88">
-        <v>0</v>
-      </c>
-      <c r="D24" s="88">
-        <v>0</v>
-      </c>
-      <c r="E24" s="88">
-        <v>0</v>
-      </c>
-      <c r="F24" s="88">
-        <v>0</v>
-      </c>
-      <c r="G24" s="88">
-        <v>0</v>
-      </c>
-      <c r="H24" s="88">
-        <v>1</v>
-      </c>
-      <c r="I24" s="88">
-        <v>1</v>
-      </c>
-      <c r="J24" s="88">
-        <v>1</v>
-      </c>
-      <c r="K24" s="88">
-        <v>1</v>
-      </c>
-      <c r="L24" s="88">
-        <v>0</v>
-      </c>
-      <c r="M24" s="88">
-        <v>0</v>
-      </c>
-      <c r="N24" s="88">
-        <v>0</v>
-      </c>
-      <c r="O24" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="52"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="89"/>
-      <c r="I25" s="89"/>
-      <c r="J25" s="89"/>
-      <c r="K25" s="89"/>
-      <c r="L25" s="89"/>
-      <c r="M25" s="89"/>
-      <c r="N25" s="89"/>
-      <c r="O25" s="89"/>
-    </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="56" t="s">
+      <c r="C25" s="88">
+        <v>0</v>
+      </c>
+      <c r="D25" s="88">
+        <v>0</v>
+      </c>
+      <c r="E25" s="88">
+        <v>0</v>
+      </c>
+      <c r="F25" s="88">
+        <v>0</v>
+      </c>
+      <c r="G25" s="88">
+        <v>0</v>
+      </c>
+      <c r="H25" s="88">
+        <v>1</v>
+      </c>
+      <c r="I25" s="88">
+        <v>1</v>
+      </c>
+      <c r="J25" s="88">
+        <v>1</v>
+      </c>
+      <c r="K25" s="88">
+        <v>1</v>
+      </c>
+      <c r="L25" s="88">
+        <v>0</v>
+      </c>
+      <c r="M25" s="88">
+        <v>0</v>
+      </c>
+      <c r="N25" s="88">
+        <v>0</v>
+      </c>
+      <c r="O25" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="52"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="89"/>
+      <c r="N26" s="89"/>
+      <c r="O26" s="89"/>
+    </row>
+    <row r="27" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B27" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="88">
-        <v>0</v>
-      </c>
-      <c r="D26" s="88">
-        <v>0</v>
-      </c>
-      <c r="E26" s="88">
-        <v>0</v>
-      </c>
-      <c r="F26" s="88">
-        <v>0</v>
-      </c>
-      <c r="G26" s="88">
-        <v>0</v>
-      </c>
-      <c r="H26" s="88">
-        <v>0</v>
-      </c>
-      <c r="I26" s="88">
-        <v>0</v>
-      </c>
-      <c r="J26" s="88">
-        <v>0</v>
-      </c>
-      <c r="K26" s="88">
-        <v>0</v>
-      </c>
-      <c r="L26" s="88">
-        <v>1</v>
-      </c>
-      <c r="M26" s="88">
-        <v>0</v>
-      </c>
-      <c r="N26" s="88">
-        <v>0</v>
-      </c>
-      <c r="O26" s="88">
-        <v>0</v>
-      </c>
-      <c r="P26" s="92"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="59" t="s">
+      <c r="C27" s="88">
+        <v>0</v>
+      </c>
+      <c r="D27" s="88">
+        <v>0</v>
+      </c>
+      <c r="E27" s="88">
+        <v>0</v>
+      </c>
+      <c r="F27" s="88">
+        <v>0</v>
+      </c>
+      <c r="G27" s="88">
+        <v>0</v>
+      </c>
+      <c r="H27" s="88">
+        <v>0</v>
+      </c>
+      <c r="I27" s="88">
+        <v>0</v>
+      </c>
+      <c r="J27" s="88">
+        <v>0</v>
+      </c>
+      <c r="K27" s="88">
+        <v>0</v>
+      </c>
+      <c r="L27" s="88">
+        <v>1</v>
+      </c>
+      <c r="M27" s="88">
+        <v>0</v>
+      </c>
+      <c r="N27" s="88">
+        <v>0</v>
+      </c>
+      <c r="O27" s="88">
+        <v>0</v>
+      </c>
+      <c r="P27" s="92"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="88">
-        <v>0</v>
-      </c>
-      <c r="D27" s="88">
-        <v>0</v>
-      </c>
-      <c r="E27" s="88">
-        <v>0</v>
-      </c>
-      <c r="F27" s="88">
-        <v>0</v>
-      </c>
-      <c r="G27" s="88">
-        <v>0</v>
-      </c>
-      <c r="H27" s="88">
-        <v>0</v>
-      </c>
-      <c r="I27" s="88">
-        <v>0</v>
-      </c>
-      <c r="J27" s="88">
-        <v>0</v>
-      </c>
-      <c r="K27" s="88">
-        <v>0</v>
-      </c>
-      <c r="L27" s="88">
-        <v>1</v>
-      </c>
-      <c r="M27" s="88">
-        <v>1</v>
-      </c>
-      <c r="N27" s="88">
-        <v>1</v>
-      </c>
-      <c r="O27" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
-      <c r="B28" s="59" t="s">
+      <c r="C28" s="88">
+        <v>0</v>
+      </c>
+      <c r="D28" s="88">
+        <v>0</v>
+      </c>
+      <c r="E28" s="88">
+        <v>0</v>
+      </c>
+      <c r="F28" s="88">
+        <v>0</v>
+      </c>
+      <c r="G28" s="88">
+        <v>0</v>
+      </c>
+      <c r="H28" s="88">
+        <v>0</v>
+      </c>
+      <c r="I28" s="88">
+        <v>0</v>
+      </c>
+      <c r="J28" s="88">
+        <v>0</v>
+      </c>
+      <c r="K28" s="88">
+        <v>0</v>
+      </c>
+      <c r="L28" s="88">
+        <v>1</v>
+      </c>
+      <c r="M28" s="88">
+        <v>1</v>
+      </c>
+      <c r="N28" s="88">
+        <v>1</v>
+      </c>
+      <c r="O28" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="56"/>
+      <c r="B29" s="59" t="s">
         <v>207</v>
-      </c>
-      <c r="C28" s="88">
-        <v>0</v>
-      </c>
-      <c r="D28" s="88">
-        <v>0</v>
-      </c>
-      <c r="E28" s="88">
-        <v>0</v>
-      </c>
-      <c r="F28" s="88">
-        <v>0</v>
-      </c>
-      <c r="G28" s="88">
-        <v>0</v>
-      </c>
-      <c r="H28" s="88">
-        <v>0</v>
-      </c>
-      <c r="I28" s="88">
-        <v>0</v>
-      </c>
-      <c r="J28" s="88">
-        <v>0</v>
-      </c>
-      <c r="K28" s="88">
-        <v>0</v>
-      </c>
-      <c r="L28" s="88">
-        <v>1</v>
-      </c>
-      <c r="M28" s="88">
-        <v>1</v>
-      </c>
-      <c r="N28" s="88">
-        <v>1</v>
-      </c>
-      <c r="O28" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="59" t="s">
-        <v>189</v>
       </c>
       <c r="C29" s="88">
         <v>0</v>
@@ -8913,114 +8913,114 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="88">
+        <v>0</v>
+      </c>
+      <c r="D30" s="88">
+        <v>0</v>
+      </c>
+      <c r="E30" s="88">
+        <v>0</v>
+      </c>
+      <c r="F30" s="88">
+        <v>0</v>
+      </c>
+      <c r="G30" s="88">
+        <v>0</v>
+      </c>
+      <c r="H30" s="88">
+        <v>0</v>
+      </c>
+      <c r="I30" s="88">
+        <v>0</v>
+      </c>
+      <c r="J30" s="88">
+        <v>0</v>
+      </c>
+      <c r="K30" s="88">
+        <v>0</v>
+      </c>
+      <c r="L30" s="88">
+        <v>1</v>
+      </c>
+      <c r="M30" s="88">
+        <v>1</v>
+      </c>
+      <c r="N30" s="88">
+        <v>1</v>
+      </c>
+      <c r="O30" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="88">
-        <v>0</v>
-      </c>
-      <c r="D30" s="88">
-        <v>0</v>
-      </c>
-      <c r="E30" s="88">
-        <v>0</v>
-      </c>
-      <c r="F30" s="88">
-        <v>0</v>
-      </c>
-      <c r="G30" s="88">
-        <v>0</v>
-      </c>
-      <c r="H30" s="88">
-        <v>0</v>
-      </c>
-      <c r="I30" s="88">
-        <v>0</v>
-      </c>
-      <c r="J30" s="88">
-        <v>0</v>
-      </c>
-      <c r="K30" s="88">
-        <v>0</v>
-      </c>
-      <c r="L30" s="88">
-        <v>1</v>
-      </c>
-      <c r="M30" s="88">
-        <v>0</v>
-      </c>
-      <c r="N30" s="88">
-        <v>0</v>
-      </c>
-      <c r="O30" s="88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="52"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="94"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
-      <c r="M31" s="89"/>
-      <c r="N31" s="89"/>
-      <c r="O31" s="89"/>
+      <c r="C31" s="88">
+        <v>0</v>
+      </c>
+      <c r="D31" s="88">
+        <v>0</v>
+      </c>
+      <c r="E31" s="88">
+        <v>0</v>
+      </c>
+      <c r="F31" s="88">
+        <v>0</v>
+      </c>
+      <c r="G31" s="88">
+        <v>0</v>
+      </c>
+      <c r="H31" s="88">
+        <v>0</v>
+      </c>
+      <c r="I31" s="88">
+        <v>0</v>
+      </c>
+      <c r="J31" s="88">
+        <v>0</v>
+      </c>
+      <c r="K31" s="88">
+        <v>0</v>
+      </c>
+      <c r="L31" s="88">
+        <v>1</v>
+      </c>
+      <c r="M31" s="88">
+        <v>0</v>
+      </c>
+      <c r="N31" s="88">
+        <v>0</v>
+      </c>
+      <c r="O31" s="88">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="56" t="s">
+      <c r="B32" s="52"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="89"/>
+      <c r="O32" s="89"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="52" t="s">
+      <c r="B33" s="52" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" s="88">
-        <v>1</v>
-      </c>
-      <c r="D32" s="88">
-        <v>0</v>
-      </c>
-      <c r="E32" s="88">
-        <v>1</v>
-      </c>
-      <c r="F32" s="88">
-        <v>1</v>
-      </c>
-      <c r="G32" s="88">
-        <v>1</v>
-      </c>
-      <c r="H32" s="88">
-        <v>1</v>
-      </c>
-      <c r="I32" s="88">
-        <v>1</v>
-      </c>
-      <c r="J32" s="88">
-        <v>1</v>
-      </c>
-      <c r="K32" s="88">
-        <v>1</v>
-      </c>
-      <c r="L32" s="88">
-        <v>1</v>
-      </c>
-      <c r="M32" s="88">
-        <v>1</v>
-      </c>
-      <c r="N32" s="88">
-        <v>1</v>
-      </c>
-      <c r="O32" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="52" t="s">
-        <v>64</v>
       </c>
       <c r="C33" s="88">
         <v>1</v>
@@ -9064,7 +9064,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" s="88">
         <v>1</v>
@@ -9108,7 +9108,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="52" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C35" s="88">
         <v>1</v>
@@ -9152,96 +9152,96 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="88">
+        <v>1</v>
+      </c>
+      <c r="D36" s="88">
+        <v>0</v>
+      </c>
+      <c r="E36" s="88">
+        <v>1</v>
+      </c>
+      <c r="F36" s="88">
+        <v>1</v>
+      </c>
+      <c r="G36" s="88">
+        <v>1</v>
+      </c>
+      <c r="H36" s="88">
+        <v>1</v>
+      </c>
+      <c r="I36" s="88">
+        <v>1</v>
+      </c>
+      <c r="J36" s="88">
+        <v>1</v>
+      </c>
+      <c r="K36" s="88">
+        <v>1</v>
+      </c>
+      <c r="L36" s="88">
+        <v>1</v>
+      </c>
+      <c r="M36" s="88">
+        <v>1</v>
+      </c>
+      <c r="N36" s="88">
+        <v>1</v>
+      </c>
+      <c r="O36" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="88">
-        <v>1</v>
-      </c>
-      <c r="D36" s="88">
-        <v>1</v>
-      </c>
-      <c r="E36" s="88">
-        <v>1</v>
-      </c>
-      <c r="F36" s="88">
-        <v>1</v>
-      </c>
-      <c r="G36" s="88">
-        <v>1</v>
-      </c>
-      <c r="H36" s="88">
-        <v>1</v>
-      </c>
-      <c r="I36" s="88">
-        <v>1</v>
-      </c>
-      <c r="J36" s="88">
-        <v>1</v>
-      </c>
-      <c r="K36" s="88">
-        <v>1</v>
-      </c>
-      <c r="L36" s="88">
-        <v>1</v>
-      </c>
-      <c r="M36" s="88">
-        <v>1</v>
-      </c>
-      <c r="N36" s="88">
-        <v>1</v>
-      </c>
-      <c r="O36" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="95"/>
-      <c r="B37" s="52" t="s">
+      <c r="C37" s="88">
+        <v>1</v>
+      </c>
+      <c r="D37" s="88">
+        <v>1</v>
+      </c>
+      <c r="E37" s="88">
+        <v>1</v>
+      </c>
+      <c r="F37" s="88">
+        <v>1</v>
+      </c>
+      <c r="G37" s="88">
+        <v>1</v>
+      </c>
+      <c r="H37" s="88">
+        <v>1</v>
+      </c>
+      <c r="I37" s="88">
+        <v>1</v>
+      </c>
+      <c r="J37" s="88">
+        <v>1</v>
+      </c>
+      <c r="K37" s="88">
+        <v>1</v>
+      </c>
+      <c r="L37" s="88">
+        <v>1</v>
+      </c>
+      <c r="M37" s="88">
+        <v>1</v>
+      </c>
+      <c r="N37" s="88">
+        <v>1</v>
+      </c>
+      <c r="O37" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="95"/>
+      <c r="B38" s="52" t="s">
         <v>83</v>
-      </c>
-      <c r="C37" s="88">
-        <v>1</v>
-      </c>
-      <c r="D37" s="88">
-        <v>1</v>
-      </c>
-      <c r="E37" s="88">
-        <v>1</v>
-      </c>
-      <c r="F37" s="88">
-        <v>1</v>
-      </c>
-      <c r="G37" s="88">
-        <v>1</v>
-      </c>
-      <c r="H37" s="88">
-        <v>1</v>
-      </c>
-      <c r="I37" s="88">
-        <v>1</v>
-      </c>
-      <c r="J37" s="88">
-        <v>1</v>
-      </c>
-      <c r="K37" s="88">
-        <v>1</v>
-      </c>
-      <c r="L37" s="88">
-        <v>1</v>
-      </c>
-      <c r="M37" s="88">
-        <v>1</v>
-      </c>
-      <c r="N37" s="88">
-        <v>1</v>
-      </c>
-      <c r="O37" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="52" t="s">
-        <v>82</v>
       </c>
       <c r="C38" s="88">
         <v>1</v>
@@ -9285,7 +9285,7 @@
     </row>
     <row r="39" spans="1:15" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" s="88">
         <v>1</v>
@@ -9329,94 +9329,138 @@
     </row>
     <row r="40" spans="1:15" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="88">
+        <v>1</v>
+      </c>
+      <c r="D40" s="88">
+        <v>1</v>
+      </c>
+      <c r="E40" s="88">
+        <v>1</v>
+      </c>
+      <c r="F40" s="88">
+        <v>1</v>
+      </c>
+      <c r="G40" s="88">
+        <v>1</v>
+      </c>
+      <c r="H40" s="88">
+        <v>1</v>
+      </c>
+      <c r="I40" s="88">
+        <v>1</v>
+      </c>
+      <c r="J40" s="88">
+        <v>1</v>
+      </c>
+      <c r="K40" s="88">
+        <v>1</v>
+      </c>
+      <c r="L40" s="88">
+        <v>1</v>
+      </c>
+      <c r="M40" s="88">
+        <v>1</v>
+      </c>
+      <c r="N40" s="88">
+        <v>1</v>
+      </c>
+      <c r="O40" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="95" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="88">
-        <v>1</v>
-      </c>
-      <c r="D40" s="88">
-        <v>1</v>
-      </c>
-      <c r="E40" s="88">
-        <v>1</v>
-      </c>
-      <c r="F40" s="88">
-        <v>1</v>
-      </c>
-      <c r="G40" s="88">
-        <v>1</v>
-      </c>
-      <c r="H40" s="88">
-        <v>1</v>
-      </c>
-      <c r="I40" s="88">
-        <v>1</v>
-      </c>
-      <c r="J40" s="88">
-        <v>1</v>
-      </c>
-      <c r="K40" s="88">
-        <v>1</v>
-      </c>
-      <c r="L40" s="88">
-        <v>1</v>
-      </c>
-      <c r="M40" s="88">
-        <v>1</v>
-      </c>
-      <c r="N40" s="88">
-        <v>1</v>
-      </c>
-      <c r="O40" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="52" t="s">
+      <c r="C41" s="88">
+        <v>1</v>
+      </c>
+      <c r="D41" s="88">
+        <v>1</v>
+      </c>
+      <c r="E41" s="88">
+        <v>1</v>
+      </c>
+      <c r="F41" s="88">
+        <v>1</v>
+      </c>
+      <c r="G41" s="88">
+        <v>1</v>
+      </c>
+      <c r="H41" s="88">
+        <v>1</v>
+      </c>
+      <c r="I41" s="88">
+        <v>1</v>
+      </c>
+      <c r="J41" s="88">
+        <v>1</v>
+      </c>
+      <c r="K41" s="88">
+        <v>1</v>
+      </c>
+      <c r="L41" s="88">
+        <v>1</v>
+      </c>
+      <c r="M41" s="88">
+        <v>1</v>
+      </c>
+      <c r="N41" s="88">
+        <v>1</v>
+      </c>
+      <c r="O41" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="88">
-        <v>1</v>
-      </c>
-      <c r="D41" s="88">
-        <v>1</v>
-      </c>
-      <c r="E41" s="88">
-        <v>1</v>
-      </c>
-      <c r="F41" s="88">
-        <v>1</v>
-      </c>
-      <c r="G41" s="88">
-        <v>1</v>
-      </c>
-      <c r="H41" s="88">
-        <v>1</v>
-      </c>
-      <c r="I41" s="88">
-        <v>1</v>
-      </c>
-      <c r="J41" s="88">
-        <v>1</v>
-      </c>
-      <c r="K41" s="88">
-        <v>1</v>
-      </c>
-      <c r="L41" s="88">
-        <v>1</v>
-      </c>
-      <c r="M41" s="88">
-        <v>1</v>
-      </c>
-      <c r="N41" s="88">
-        <v>1</v>
-      </c>
-      <c r="O41" s="88">
+      <c r="C42" s="88">
+        <v>1</v>
+      </c>
+      <c r="D42" s="88">
+        <v>1</v>
+      </c>
+      <c r="E42" s="88">
+        <v>1</v>
+      </c>
+      <c r="F42" s="88">
+        <v>1</v>
+      </c>
+      <c r="G42" s="88">
+        <v>1</v>
+      </c>
+      <c r="H42" s="88">
+        <v>1</v>
+      </c>
+      <c r="I42" s="88">
+        <v>1</v>
+      </c>
+      <c r="J42" s="88">
+        <v>1</v>
+      </c>
+      <c r="K42" s="88">
+        <v>1</v>
+      </c>
+      <c r="L42" s="88">
+        <v>1</v>
+      </c>
+      <c r="M42" s="88">
+        <v>1</v>
+      </c>
+      <c r="N42" s="88">
+        <v>1</v>
+      </c>
+      <c r="O42" s="88">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UTAD6hDPFf/Ul0P2TkEmcVLwJIskng6BwO7PQn9KQppd8AxlpMXDzh2uUA/A2vdLAdLHbrkvLJZl/FHFHl0BRA==" saltValue="WyzBb18fC4LyksUq9iofgA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dM4uje+9RyuRxxJKnHAouYPb4///Rtb5SimwoPIpJuy0NanxiYtwY96RXZmiRHdHpR5udqKR1eqcfxMDzk0QSQ==" saltValue="18UcNHkjNKYPMZLpFhWkwg==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9428,7 +9472,7 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -9482,7 +9526,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
@@ -9499,7 +9543,7 @@
       <c r="J2" s="88"/>
       <c r="K2" s="88"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>86</v>
       </c>
@@ -9516,7 +9560,7 @@
       <c r="J3" s="88"/>
       <c r="K3" s="88"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>61</v>
       </c>
@@ -9533,7 +9577,7 @@
       <c r="J4" s="88"/>
       <c r="K4" s="88"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>149</v>
       </c>
@@ -9550,7 +9594,7 @@
       <c r="J5" s="88"/>
       <c r="K5" s="88"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>197</v>
       </c>
@@ -9569,7 +9613,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>63</v>
       </c>
@@ -9588,7 +9632,7 @@
       <c r="J7" s="88"/>
       <c r="K7" s="88"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>64</v>
       </c>
@@ -9607,7 +9651,7 @@
       <c r="J8" s="88"/>
       <c r="K8" s="88"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>62</v>
       </c>
@@ -9626,7 +9670,7 @@
       <c r="J9" s="88"/>
       <c r="K9" s="88"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
         <v>188</v>
       </c>
@@ -9643,7 +9687,7 @@
       <c r="J10" s="88"/>
       <c r="K10" s="88"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
         <v>207</v>
       </c>
@@ -9660,7 +9704,7 @@
       <c r="J11" s="88"/>
       <c r="K11" s="88"/>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
         <v>189</v>
       </c>
@@ -9677,7 +9721,7 @@
       <c r="J12" s="88"/>
       <c r="K12" s="88"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
         <v>190</v>
       </c>
@@ -9694,7 +9738,7 @@
       <c r="J13" s="88"/>
       <c r="K13" s="88"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>187</v>
       </c>
@@ -9713,7 +9757,7 @@
       <c r="J14" s="88"/>
       <c r="K14" s="88"/>
     </row>
-    <row r="15" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>208</v>
       </c>
@@ -9732,7 +9776,7 @@
       <c r="J15" s="88"/>
       <c r="K15" s="88"/>
     </row>
-    <row r="16" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>57</v>
       </c>
@@ -9753,7 +9797,7 @@
       <c r="J16" s="88"/>
       <c r="K16" s="88"/>
     </row>
-    <row r="17" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>47</v>
       </c>
@@ -9770,7 +9814,7 @@
       <c r="J17" s="88"/>
       <c r="K17" s="88"/>
     </row>
-    <row r="18" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>173</v>
       </c>
@@ -9789,7 +9833,7 @@
       <c r="J18" s="88"/>
       <c r="K18" s="88"/>
     </row>
-    <row r="19" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>198</v>
       </c>
@@ -9808,7 +9852,7 @@
       <c r="J19" s="88"/>
       <c r="K19" s="88"/>
     </row>
-    <row r="20" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
         <v>199</v>
       </c>
@@ -9827,7 +9871,7 @@
       <c r="J20" s="88"/>
       <c r="K20" s="88"/>
     </row>
-    <row r="21" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>195</v>
       </c>
@@ -9846,7 +9890,7 @@
       <c r="J21" s="88"/>
       <c r="K21" s="88"/>
     </row>
-    <row r="22" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
         <v>136</v>
       </c>
@@ -9867,7 +9911,7 @@
       <c r="J22" s="88"/>
       <c r="K22" s="88"/>
     </row>
-    <row r="23" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>34</v>
       </c>
@@ -10245,7 +10289,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -10274,7 +10318,7 @@
       <c r="J2" s="88"/>
       <c r="K2" s="88"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -10303,7 +10347,7 @@
       <c r="J3" s="88"/>
       <c r="K3" s="88"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -10332,7 +10376,7 @@
       <c r="J4" s="88"/>
       <c r="K4" s="88"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
@@ -10361,7 +10405,7 @@
       <c r="J5" s="88"/>
       <c r="K5" s="88"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
@@ -10390,7 +10434,7 @@
       <c r="J6" s="88"/>
       <c r="K6" s="88"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>53</v>
       </c>
@@ -10411,7 +10455,7 @@
       <c r="J7" s="88"/>
       <c r="K7" s="88"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>54</v>
       </c>
@@ -10432,7 +10476,7 @@
       <c r="J8" s="88"/>
       <c r="K8" s="88"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>55</v>
       </c>
@@ -10453,7 +10497,7 @@
       <c r="J9" s="88"/>
       <c r="K9" s="88"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
@@ -10474,7 +10518,7 @@
       <c r="J10" s="88"/>
       <c r="K10" s="88"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>49</v>
       </c>
@@ -10495,7 +10539,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>50</v>
       </c>
@@ -10514,7 +10558,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>51</v>
       </c>
@@ -10533,7 +10577,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>52</v>
       </c>
@@ -10607,7 +10651,7 @@
       <c r="A2" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="139" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -10629,8 +10673,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="135"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="139"/>
       <c r="C3" s="35" t="s">
         <v>175</v>
       </c>
@@ -10651,8 +10695,8 @@
       </c>
       <c r="J3" s="98"/>
     </row>
-    <row r="4" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="135"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="139"/>
       <c r="C4" s="35" t="s">
         <v>174</v>
       </c>
@@ -10673,8 +10717,8 @@
       </c>
       <c r="J4" s="98"/>
     </row>
-    <row r="5" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="135" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="139" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="35" t="s">
@@ -10697,8 +10741,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="135"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="139"/>
       <c r="C6" s="35" t="s">
         <v>175</v>
       </c>
@@ -10718,8 +10762,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="135"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="139"/>
       <c r="C7" s="35" t="s">
         <v>174</v>
       </c>
@@ -10739,8 +10783,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="135" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="139" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -10762,8 +10806,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="135"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="139"/>
       <c r="C9" s="35" t="s">
         <v>175</v>
       </c>
@@ -10783,8 +10827,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="135"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="139"/>
       <c r="C10" s="35" t="s">
         <v>174</v>
       </c>
@@ -10804,8 +10848,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="135" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="139" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="35" t="s">
@@ -10827,8 +10871,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="135"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="139"/>
       <c r="C12" s="35" t="s">
         <v>175</v>
       </c>
@@ -10848,8 +10892,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="135"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="139"/>
       <c r="C13" s="35" t="s">
         <v>174</v>
       </c>
@@ -10869,8 +10913,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="135" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="139" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
@@ -10892,8 +10936,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="135"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="139"/>
       <c r="C15" s="35" t="s">
         <v>175</v>
       </c>
@@ -10913,8 +10957,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="135"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="139"/>
       <c r="C16" s="35" t="s">
         <v>174</v>
       </c>
@@ -10957,7 +11001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
       <c r="F18" s="100"/>
@@ -10968,7 +11012,7 @@
       <c r="A19" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="B19" s="135" t="s">
+      <c r="B19" s="139" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="35" t="s">
@@ -10990,8 +11034,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="135"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="139"/>
       <c r="C20" s="35" t="s">
         <v>175</v>
       </c>
@@ -11011,8 +11055,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="135"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="139"/>
       <c r="C21" s="35" t="s">
         <v>174</v>
       </c>
@@ -11032,8 +11076,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="135" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="139" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="35" t="s">
@@ -11055,8 +11099,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="135"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="139"/>
       <c r="C23" s="35" t="s">
         <v>175</v>
       </c>
@@ -11076,8 +11120,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="135"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="139"/>
       <c r="C24" s="35" t="s">
         <v>174</v>
       </c>
@@ -11097,8 +11141,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="135" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="139" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="35" t="s">
@@ -11120,8 +11164,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="135"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="139"/>
       <c r="C26" s="35" t="s">
         <v>175</v>
       </c>
@@ -11141,8 +11185,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="135"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="139"/>
       <c r="C27" s="35" t="s">
         <v>174</v>
       </c>
@@ -11162,8 +11206,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="135" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="139" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="35" t="s">
@@ -11186,7 +11230,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="135"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="35" t="s">
         <v>175</v>
       </c>
@@ -11207,7 +11251,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="135"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="35" t="s">
         <v>174</v>
       </c>
@@ -11228,7 +11272,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="135" t="s">
+      <c r="B31" s="139" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="35" t="s">
@@ -11251,7 +11295,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="135"/>
+      <c r="B32" s="139"/>
       <c r="C32" s="35" t="s">
         <v>175</v>
       </c>
@@ -11272,7 +11316,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="135"/>
+      <c r="B33" s="139"/>
       <c r="C33" s="35" t="s">
         <v>174</v>
       </c>
@@ -11326,7 +11370,7 @@
       <c r="A36" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="B36" s="135" t="s">
+      <c r="B36" s="139" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="35" t="s">
@@ -11349,7 +11393,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="135"/>
+      <c r="B37" s="139"/>
       <c r="C37" s="35" t="s">
         <v>175</v>
       </c>
@@ -11370,7 +11414,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="135"/>
+      <c r="B38" s="139"/>
       <c r="C38" s="35" t="s">
         <v>174</v>
       </c>
@@ -11391,7 +11435,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="135" t="s">
+      <c r="B39" s="139" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="35" t="s">
@@ -11414,7 +11458,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="135"/>
+      <c r="B40" s="139"/>
       <c r="C40" s="35" t="s">
         <v>175</v>
       </c>
@@ -11435,7 +11479,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="135"/>
+      <c r="B41" s="139"/>
       <c r="C41" s="35" t="s">
         <v>174</v>
       </c>
@@ -11456,7 +11500,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="135" t="s">
+      <c r="B42" s="139" t="s">
         <v>2</v>
       </c>
       <c r="C42" s="35" t="s">
@@ -11479,7 +11523,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="135"/>
+      <c r="B43" s="139"/>
       <c r="C43" s="35" t="s">
         <v>175</v>
       </c>
@@ -11500,7 +11544,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="135"/>
+      <c r="B44" s="139"/>
       <c r="C44" s="35" t="s">
         <v>174</v>
       </c>
@@ -11521,7 +11565,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="139" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="35" t="s">
@@ -11544,7 +11588,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="135"/>
+      <c r="B46" s="139"/>
       <c r="C46" s="35" t="s">
         <v>175</v>
       </c>
@@ -11565,7 +11609,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="135"/>
+      <c r="B47" s="139"/>
       <c r="C47" s="35" t="s">
         <v>174</v>
       </c>
@@ -11586,7 +11630,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="135" t="s">
+      <c r="B48" s="139" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="35" t="s">
@@ -11609,7 +11653,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="135"/>
+      <c r="B49" s="139"/>
       <c r="C49" s="35" t="s">
         <v>175</v>
       </c>
@@ -11630,7 +11674,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="135"/>
+      <c r="B50" s="139"/>
       <c r="C50" s="35" t="s">
         <v>174</v>
       </c>
@@ -11676,6 +11720,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11685,12 +11735,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -17521,7 +17565,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="59" t="s">
         <v>67</v>
       </c>
@@ -17552,7 +17596,7 @@
       <c r="F4" s="133"/>
       <c r="G4" s="133"/>
     </row>
-    <row r="5" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="90" t="s">
         <v>183</v>
       </c>
@@ -17629,7 +17673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
@@ -17655,7 +17699,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="52" t="s">
         <v>268</v>
       </c>
@@ -17675,7 +17719,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="52" t="s">
         <v>269</v>
       </c>
@@ -17695,7 +17739,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>58</v>
       </c>
@@ -17721,7 +17765,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="52" t="s">
         <v>269</v>
       </c>
@@ -17741,7 +17785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>65</v>
       </c>
@@ -17764,7 +17808,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="52" t="s">
         <v>269</v>
       </c>
@@ -17784,7 +17828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>136</v>
       </c>
@@ -17810,7 +17854,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="52" t="s">
         <v>269</v>
       </c>
@@ -17830,7 +17874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
         <v>65</v>
       </c>
@@ -17853,7 +17897,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
         <v>269</v>
       </c>
@@ -17873,7 +17917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>61</v>
       </c>
@@ -17899,7 +17943,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="52" t="s">
         <v>269</v>
       </c>
@@ -17920,7 +17964,7 @@
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
         <v>65</v>
       </c>
@@ -17944,7 +17988,7 @@
       </c>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
         <v>269</v>
       </c>
@@ -17965,7 +18009,7 @@
       </c>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>62</v>
       </c>
@@ -17992,7 +18036,7 @@
       </c>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
         <v>268</v>
       </c>
@@ -18013,7 +18057,7 @@
       </c>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>63</v>
       </c>
@@ -18039,7 +18083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="52" t="s">
         <v>268</v>
       </c>
@@ -18059,7 +18103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>64</v>
       </c>
@@ -18085,7 +18129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" s="52" t="s">
         <v>268</v>
       </c>
@@ -18105,7 +18149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>79</v>
       </c>
@@ -18131,7 +18175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="52" t="s">
         <v>268</v>
       </c>
@@ -18151,7 +18195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="52" t="s">
         <v>269</v>
       </c>
@@ -18171,7 +18215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>80</v>
       </c>
@@ -18197,7 +18241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="52" t="s">
         <v>268</v>
       </c>
@@ -18217,7 +18261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="52" t="s">
         <v>269</v>
       </c>
@@ -18237,7 +18281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>81</v>
       </c>
@@ -18263,7 +18307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="52" t="s">
         <v>268</v>
       </c>
@@ -18283,7 +18327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="52" t="s">
         <v>269</v>
       </c>
@@ -18303,7 +18347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>82</v>
       </c>
@@ -18329,7 +18373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="52" t="s">
         <v>268</v>
       </c>
@@ -18349,7 +18393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="52" t="s">
         <v>269</v>
       </c>
@@ -18369,7 +18413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>83</v>
       </c>
@@ -18395,7 +18439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="52" t="s">
         <v>268</v>
       </c>
@@ -18415,7 +18459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="52" t="s">
         <v>269</v>
       </c>
@@ -18435,7 +18479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>60</v>
       </c>
@@ -18461,7 +18505,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="52" t="s">
         <v>268</v>
       </c>
@@ -18481,7 +18525,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="52" t="s">
         <v>269</v>
       </c>
@@ -18501,7 +18545,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="52" t="s">
         <v>16</v>
       </c>
@@ -18524,7 +18568,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="52" t="s">
         <v>268</v>
       </c>
@@ -18544,7 +18588,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="52" t="s">
         <v>269</v>
       </c>
@@ -18564,7 +18608,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
         <v>84</v>
       </c>
@@ -18590,7 +18634,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="52" t="s">
         <v>268</v>
       </c>
@@ -18610,7 +18654,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
         <v>85</v>
       </c>
@@ -18636,7 +18680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="52" t="s">
         <v>268</v>
       </c>
@@ -18656,7 +18700,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
         <v>195</v>
       </c>
@@ -18751,7 +18795,7 @@
       </c>
       <c r="H1" s="96"/>
     </row>
-    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>86</v>
       </c>
@@ -18775,7 +18819,7 @@
       </c>
       <c r="H2" s="90"/>
     </row>
-    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="35" t="s">
         <v>268</v>
       </c>
@@ -18793,7 +18837,7 @@
       </c>
       <c r="H3" s="134"/>
     </row>
-    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>87</v>
       </c>
@@ -18817,7 +18861,7 @@
       </c>
       <c r="H4" s="134"/>
     </row>
-    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="C5" s="35" t="s">
         <v>268</v>
@@ -18836,7 +18880,7 @@
       </c>
       <c r="H5" s="90"/>
     </row>
-    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>88</v>
       </c>
@@ -18860,7 +18904,7 @@
       </c>
       <c r="H6" s="90"/>
     </row>
-    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="C7" s="35" t="s">
         <v>268</v>
@@ -19939,7 +19983,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -19956,10 +20000,10 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -19976,10 +20020,10 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -19996,7 +20040,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
@@ -20010,7 +20054,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
@@ -20024,7 +20068,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -20041,7 +20085,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
@@ -20055,7 +20099,7 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
@@ -20072,7 +20116,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
@@ -20142,7 +20186,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="46" t="s">
         <v>1</v>
@@ -20156,7 +20200,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="46" t="s">
         <v>2</v>
@@ -20170,7 +20214,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="46" t="s">
         <v>3</v>
@@ -20184,7 +20228,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="46" t="s">
         <v>4</v>
@@ -20198,7 +20242,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="46" t="s">
         <v>172</v>
@@ -20223,7 +20267,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="46" t="s">
         <v>1</v>
@@ -20235,7 +20279,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="46" t="s">
         <v>2</v>
@@ -20247,7 +20291,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="46" t="s">
         <v>3</v>
@@ -20259,7 +20303,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="46" t="s">
         <v>4</v>
@@ -20271,7 +20315,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="46" t="s">
         <v>172</v>
@@ -20296,7 +20340,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="46" t="s">
         <v>1</v>
@@ -20310,7 +20354,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="46" t="s">
         <v>2</v>
@@ -20324,7 +20368,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="46" t="s">
         <v>3</v>
@@ -20338,7 +20382,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="46" t="s">
         <v>4</v>
@@ -20381,52 +20425,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="135" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="136" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="137" t="s">
+      <c r="C1" s="136" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="137" t="s">
+      <c r="D1" s="136" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="136" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="137" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="138" t="s">
+      <c r="C2" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="139"/>
+      <c r="D2" s="138"/>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="136" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="137" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="139"/>
+      <c r="D3" s="138"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="THDTDI6gFQG6sxcoBIxkeYJ0DN9sRDdt+s06ZVU7ubYruE8V3BhPB+QJswc4/26vB++Z43zP22MdKla7x+hIfg==" saltValue="XJeJAHzq9TVXeiC8frBHFg==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FjVY04+iPZ+KFsAAY50OVBgJhMmG/Eze7ERNwDiYTqpNijGKVPMn+Z7rivyvqHi2EX9g6nqNla/apcDjQLAfng==" saltValue="Wgt1Ghrmmt2XHcb32w2lmA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>